<commit_message>
Adding progress events in production namespace and pumpcontrol room closes #129
</commit_message>
<xml_diff>
--- a/socketio_interface.xlsx
+++ b/socketio_interface.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Tabelle 1</t>
   </si>
@@ -40,16 +40,28 @@
     <t>state</t>
   </si>
   <si>
-    <t>{orderNumer:…,fromState:…,toState:…}</t>
+    <t>{orderNumber:…,fromState:…,toState:…}</t>
   </si>
   <si>
     <t>The statechange of a order (on registering the room, a event with the current state (only toState) will be fired)</t>
   </si>
   <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>{orderNumber:…,progress:…}</t>
+  </si>
+  <si>
+    <t>The progress of a order (on registering the room, a event with the current progress will be fired)</t>
+  </si>
+  <si>
     <t>allOrders</t>
   </si>
   <si>
-    <t>Statechanges of all orders (on registering the room, events for all states will be fired (only toState))</t>
+    <t>Statechanges of all orders (on registering the room, events for all orders will be fired (only toState))</t>
+  </si>
+  <si>
+    <t>Progress changes or all orders (on registering the room, events for all orders will be fired)</t>
   </si>
   <si>
     <t>add</t>
@@ -107,6 +119,15 @@
   </si>
   <si>
     <t>Fired when the amount left of a component is below the configured minimum amount. warningCleared: true means the warning has been cleared</t>
+  </si>
+  <si>
+    <t>pumpControl</t>
+  </si>
+  <si>
+    <t>progress (number 0-100)</t>
+  </si>
+  <si>
+    <t>The progress from 0 to 100 of the currently relevant order.</t>
   </si>
   <si>
     <t>/connectionState</t>
@@ -128,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -136,6 +157,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -152,7 +178,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +197,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -184,6 +216,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -197,7 +251,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -206,7 +260,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -215,43 +269,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -260,28 +314,88 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -291,35 +405,50 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -339,8 +468,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -359,10 +490,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -539,11 +670,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -552,27 +686,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -829,10 +963,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1123,7 +1257,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1404,7 +1538,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1422,179 +1556,230 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" t="s" s="8">
         <v>9</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E3" t="s" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+    <row r="4" ht="20.25" customHeight="1">
+      <c r="A4" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s" s="9">
+      <c r="D4" t="s" s="12">
         <v>12</v>
+      </c>
+      <c r="E4" t="s" s="8">
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="A5" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="B5" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="9">
+      <c r="B5" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="9">
+      <c r="C5" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s" s="12">
         <v>15</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="A6" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s" s="12">
         <v>16</v>
-      </c>
-      <c r="B6" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s" s="9">
-        <v>19</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s" s="9">
-        <v>21</v>
+      <c r="A7" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="12">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s" s="12">
+        <v>19</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s" s="8">
+      <c r="A8" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s" s="12">
         <v>22</v>
       </c>
-      <c r="C8" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s" s="9">
+      <c r="E8" t="s" s="12">
         <v>23</v>
-      </c>
-      <c r="E8" t="s" s="9">
-        <v>24</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s" s="8">
+      <c r="A9" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="14">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s" s="12">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s" s="12">
         <v>25</v>
-      </c>
-      <c r="C9" t="s" s="9">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="9">
-        <v>28</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s" s="8">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s" s="9">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s" s="9">
-        <v>31</v>
+      <c r="A10" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s" s="14">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="12">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s" s="12">
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="7">
+      <c r="A11" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s" s="14">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s" s="12">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s" s="12">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s" s="12">
         <v>32</v>
       </c>
-      <c r="B11" t="s" s="8">
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="14">
         <v>33</v>
       </c>
-      <c r="C11" t="s" s="9">
+      <c r="C12" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="D11" t="s" s="9">
+      <c r="D12" t="s" s="12">
         <v>34</v>
       </c>
-      <c r="E11" t="s" s="9">
+      <c r="E12" t="s" s="12">
         <v>35</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s" s="12">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s" s="12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s" s="14">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s" s="12">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s" s="12">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>